<commit_message>
Connection via supabase added
</commit_message>
<xml_diff>
--- a/lab3/table.xlsx
+++ b/lab3/table.xlsx
@@ -2342,7 +2342,7 @@
         <v>20</v>
       </c>
       <c r="B198" t="n">
-        <v>103.0</v>
+        <v>133.0</v>
       </c>
       <c r="C198" t="n">
         <v>2014.0</v>
@@ -2353,7 +2353,7 @@
         <v>20</v>
       </c>
       <c r="B199" t="n">
-        <v>140.0</v>
+        <v>170.0</v>
       </c>
       <c r="C199" t="n">
         <v>2015.0</v>

</xml_diff>